<commit_message>
modifica grafica per leggibilità
</commit_message>
<xml_diff>
--- a/report_metodi/risultati_Static.xlsx
+++ b/report_metodi/risultati_Static.xlsx
@@ -1,37 +1,54 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\melo\Bakarà\Counting_Bakar-\report_metodi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1399DD2-8480-46C7-AE2B-EB47BA02B8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Simulazione</t>
+  </si>
+  <si>
+    <t>Bilancio_Finale</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +63,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,428 +387,422 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Simulazione</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Bilancio_Finale</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>-160</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>-120</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>20</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>-60</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>-110</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>40</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>60</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>130</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="n">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>40</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="n">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>-20</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="n">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>10</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="n">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>-130</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="n">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>-70</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="n">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>-70</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="n">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>-90</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="n">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>-50</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="n">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>50</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="n">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>20</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="n">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>-10</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="n">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>-20</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="n">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>80</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="n">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>-100</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="n">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>10</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="n">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>-40</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="n">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>60</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="n">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>30</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="n">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>120</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="n">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>-50</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="n">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>-180</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="n">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>-30</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="n">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>120</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="n">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>-110</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="n">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>40</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="n">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>-40</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="n">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>10</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="n">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>-10</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="n">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>-100</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="n">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>0</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="n">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>-20</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="n">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>-20</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="n">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>-110</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="n">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>110</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="n">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>-100</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="n">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>90</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="n">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>-210</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="n">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>-130</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="n">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>-140</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="n">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>-150</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="n">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>-60</v>
       </c>
     </row>

</xml_diff>